<commit_message>
Fixed Messenger stale data + multi-key rotation + flush fix
</commit_message>
<xml_diff>
--- a/python-projects/Plex Scraper Project/Plex_Analysis_20260217_182646.xlsx
+++ b/python-projects/Plex Scraper Project/Plex_Analysis_20260217_182646.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thorasys-my.sharepoint.com/personal/guy_drapeau_thorasys_com/Documents/Documents/CLAUDE/Plex Scraper Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thorasys-my.sharepoint.com/personal/guy_drapeau_thorasys_com/Documents/Documents/CLAUDE/python-projects/Plex Scraper Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_CA586D47CF82D714F5844AF0E78C73D30C5E25D1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BAE894B-B939-46B0-B4DC-3BE570EBD8BB}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_CA586D47CF82D714F5844AF0E78C73D30C5E25D1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D7E8324-FCDA-40AC-9F31-822B0A9B6547}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -631,7 +631,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2646,7 +2646,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2689,7 +2689,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="14" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -5444,6 +5444,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{EDE61592-6E48-47F9-84D8-4716D1EDC552}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>